<commit_message>
excel_processor.py able to process multiple sheets and giving multiple excel as output
</commit_message>
<xml_diff>
--- a/processed_sheets/cleaned_NBCE_The Voice S28_Fall_25_RFP Template (Samsung Ads) 5.13_400K_Media_Plan.xlsx
+++ b/processed_sheets/cleaned_NBCE_The Voice S28_Fall_25_RFP Template (Samsung Ads) 5.13_400K_Media_Plan.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="$400K Media Plan" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="$400K Media Plan" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,19 +52,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -470,24 +463,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -497,161 +472,157 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Site Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Package Name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Placement Name</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Audience Demo (P2+, A18-49, AA, HM)</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Audience Targeting 
 (ex: E! Network viewers, etc.)</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Device Type
 (Mobile Web, Mobile App,  Tablet, Desktop)</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Ad Unit/Size</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Site Served Only
 (Y/N)</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Buy Model</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Media Type
 (Flash, Rich Media, Video Etc.)</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>Start Date</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>End Date</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>Can be purchased on Viewability? (MOAT GroupM Viewability Standard)</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>Can Utilize MOAT on this placement?
 (Y/N)</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>Can Purchase Programmatically? (via DV 360)  (Y/N)</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="2" t="inlineStr">
         <is>
           <t>Can utilize DV on this placement?
 (Y/N)</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>AutoPlay or Click to Play?</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" s="2" t="inlineStr">
         <is>
           <t>Is the Unit Skippable, Nonskippable or blended?</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="S1" s="2" t="inlineStr">
         <is>
           <t>Creative Restrictions (# of Swaps OR # of creative versions) per Line Item (specify # and caveat if it includes tune-in messaging)</t>
         </is>
       </c>
-      <c r="T1" s="5" t="inlineStr">
+      <c r="T1" s="2" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="U1" s="5" t="inlineStr">
+      <c r="U1" s="2" t="inlineStr">
         <is>
           <t>Impressions</t>
         </is>
       </c>
-      <c r="V1" s="5" t="inlineStr">
+      <c r="V1" s="2" t="inlineStr">
         <is>
           <t>Net Cost</t>
         </is>
       </c>
-      <c r="W1" s="5" t="inlineStr">
+      <c r="W1" s="2" t="inlineStr">
         <is>
           <t>Cancellaton Date by Package</t>
         </is>
       </c>
-      <c r="X1" s="5" t="inlineStr">
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>% SOV</t>
         </is>
       </c>
-      <c r="Y1" s="5" t="inlineStr">
+      <c r="Y1" s="2" t="inlineStr">
         <is>
           <t>Minimum package/placement amount</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Samsung Ads</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>CTV</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>CTV Video_Lead-In_2016+ Models: 
 Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Target 1
 Viewers/Fans of The Voice (especially S26 and S27) + LALs:
@@ -666,124 +637,120 @@
 Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Smart TV</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>:15/:30</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>3P Tracking</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Video</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>2025-09-18 00:00:00</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>2025-10-07 00:00:00</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N2" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O2" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P2" s="5" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
         <is>
           <t>Y - Tracking Only</t>
         </is>
       </c>
-      <c r="Q2" s="5" t="inlineStr">
+      <c r="Q2" s="2" t="inlineStr">
         <is>
           <t>AutoPlay</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="R2" s="2" t="inlineStr">
         <is>
           <t>Nonskippable</t>
         </is>
       </c>
-      <c r="S2" s="5" t="inlineStr">
+      <c r="S2" s="2" t="inlineStr">
         <is>
           <t>No restrictions on # of creatives if using VAST tags</t>
         </is>
       </c>
-      <c r="T2" s="6" t="inlineStr">
+      <c r="T2" s="3" t="inlineStr">
         <is>
           <t>33.5</t>
         </is>
       </c>
-      <c r="U2" s="7">
-        <f>V2/T2*1000</f>
-        <v/>
-      </c>
-      <c r="V2" s="8" t="inlineStr">
-        <is>
-          <t>175000.0</t>
-        </is>
-      </c>
-      <c r="W2" s="5" t="inlineStr">
+      <c r="U2" s="3" t="inlineStr">
+        <is>
+          <t>5223880.597</t>
+        </is>
+      </c>
+      <c r="V2" s="4" t="inlineStr">
+        <is>
+          <t>175000</t>
+        </is>
+      </c>
+      <c r="W2" s="2" t="inlineStr">
         <is>
           <t>14 days</t>
         </is>
       </c>
-      <c r="X2" s="5">
-        <f>U53/'Max Avails'!U53</f>
-        <v/>
-      </c>
-      <c r="Y2" s="5" t="inlineStr">
+      <c r="X2" s="2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Y2" s="2" t="inlineStr">
         <is>
           <t>$10K Line Item Minimum, $75K Plan Minimum</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>First Screen Rotational</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>First Screen Rotational_Lead In_Click to Video_2017+ Models: 
 Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Target 1
 Viewers/Fans of The Voice (especially S26 and S27) + LALs:
@@ -798,125 +765,113 @@
 Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Smart TV </t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
 Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>Yes (but can be tracked by a DCM 1x1)</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>Custom Display</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="K3" s="2" t="inlineStr">
         <is>
           <t>2025-09-18 00:00:00</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>2025-09-22 00:00:00</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N3" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R3" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S3" s="5" t="inlineStr">
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
         </is>
       </c>
-      <c r="T3" s="6" t="inlineStr">
+      <c r="T3" s="3" t="inlineStr">
         <is>
           <t>14.25</t>
         </is>
       </c>
-      <c r="U3" s="7">
-        <f>V3/T3*1000</f>
-        <v/>
-      </c>
-      <c r="V3" s="8" t="inlineStr">
-        <is>
-          <t>60000.0</t>
-        </is>
-      </c>
-      <c r="W3" s="5" t="inlineStr">
+      <c r="U3" s="3" t="inlineStr">
+        <is>
+          <t>4210526.316</t>
+        </is>
+      </c>
+      <c r="V3" s="4" t="inlineStr">
+        <is>
+          <t>60000</t>
+        </is>
+      </c>
+      <c r="W3" s="2" t="inlineStr">
         <is>
           <t>14 days</t>
         </is>
       </c>
-      <c r="X3" s="5">
-        <f>U54/'Max Avails'!U54</f>
-        <v/>
-      </c>
-      <c r="Y3" s="5" t="inlineStr">
+      <c r="X3" s="2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Y3" s="2" t="inlineStr">
         <is>
           <t>$10K Line Item Minimum, $75K Plan Minimum</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n"/>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>First Screen Immersive Rotational</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>'22 First Screen Immersive_Click to Video_2022-2024 Models:
 Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Target 1
 Viewers/Fans of The Voice (especially S26 and S27) + LALs:
@@ -931,125 +886,113 @@
 Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Smart TV </t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Banner: 3840x2160
 Transparent Logo: 1120x400</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Yes (but can be tracked by a DCM 1x1)</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="J4" s="2" t="inlineStr">
         <is>
           <t>Custom Display</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="K4" s="2" t="inlineStr">
         <is>
           <t>2025-09-18 00:00:00</t>
         </is>
       </c>
-      <c r="L4" s="5" t="inlineStr">
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>2025-09-22 00:00:00</t>
         </is>
       </c>
-      <c r="M4" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N4" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O4" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P4" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Q4" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R4" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S4" s="5" t="inlineStr">
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N4" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="n"/>
+      <c r="R4" s="2" t="n"/>
+      <c r="S4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
         </is>
       </c>
-      <c r="T4" s="6" t="inlineStr">
+      <c r="T4" s="3" t="inlineStr">
         <is>
           <t>21.5</t>
         </is>
       </c>
-      <c r="U4" s="7">
-        <f>V4/T4*1000</f>
-        <v/>
-      </c>
-      <c r="V4" s="8" t="inlineStr">
-        <is>
-          <t>40000.0</t>
-        </is>
-      </c>
-      <c r="W4" s="5" t="inlineStr">
+      <c r="U4" s="3" t="inlineStr">
+        <is>
+          <t>1860465.116</t>
+        </is>
+      </c>
+      <c r="V4" s="4" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="W4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Non-cancellable, but can be shifted with a 60 days notice before launch </t>
         </is>
       </c>
-      <c r="X4" s="5">
-        <f>U55/'Max Avails'!U55</f>
-        <v/>
-      </c>
-      <c r="Y4" s="5" t="inlineStr">
+      <c r="X4" s="2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
         <is>
           <t>$10K Line Item Minimum, $75K Plan Minimum</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>First Screen Rotational</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>First Screen Rotational_Click to App_2017+ Models: 
 Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>Target 1
 Viewers/Fans of The Voice (especially S26 and S27) + LALs:
@@ -1064,125 +1007,113 @@
 Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Smart TV </t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
 Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="H5" s="2" t="inlineStr">
         <is>
           <t>Yes (but can be tracked by a DCM 1x1)</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="I5" s="2" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="J5" s="2" t="inlineStr">
         <is>
           <t>Custom Display</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="K5" s="2" t="inlineStr">
         <is>
           <t>2025-09-23 00:00:00</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="L5" s="2" t="inlineStr">
         <is>
           <t>2025-10-07 00:00:00</t>
         </is>
       </c>
-      <c r="M5" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N5" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O5" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P5" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Q5" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R5" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S5" s="5" t="inlineStr">
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N5" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q5" s="2" t="n"/>
+      <c r="R5" s="2" t="n"/>
+      <c r="S5" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
         </is>
       </c>
-      <c r="T5" s="6" t="inlineStr">
+      <c r="T5" s="3" t="inlineStr">
         <is>
           <t>14.25</t>
         </is>
       </c>
-      <c r="U5" s="7">
-        <f>V5/T5*1000</f>
-        <v/>
-      </c>
-      <c r="V5" s="8" t="inlineStr">
-        <is>
-          <t>75000.0</t>
-        </is>
-      </c>
-      <c r="W5" s="5" t="inlineStr">
+      <c r="U5" s="3" t="inlineStr">
+        <is>
+          <t>5263157.895</t>
+        </is>
+      </c>
+      <c r="V5" s="4" t="inlineStr">
+        <is>
+          <t>75000</t>
+        </is>
+      </c>
+      <c r="W5" s="2" t="inlineStr">
         <is>
           <t>14 days</t>
         </is>
       </c>
-      <c r="X5" s="5">
-        <f>U56/'Max Avails'!U57</f>
-        <v/>
-      </c>
-      <c r="Y5" s="5" t="inlineStr">
+      <c r="X5" s="2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Y5" s="2" t="inlineStr">
         <is>
           <t>$10K Line Item Minimum, $75K Plan Minimum</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n"/>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>First Screen Immersive Rotational</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>'22 First Screen Immersive_Click to App_2022-2024 Models:
 Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Target 1
 Viewers/Fans of The Voice (especially S26 and S27) + LALs:
@@ -1197,114 +1128,106 @@
 Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Smart TV </t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>Banner: 3840x2160
 Transparent Logo: 1120x400</t>
         </is>
       </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>Yes (but can be tracked by a DCM 1x1)</t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="J6" s="2" t="inlineStr">
         <is>
           <t>Custom Display</t>
         </is>
       </c>
-      <c r="K6" s="5" t="inlineStr">
+      <c r="K6" s="2" t="inlineStr">
         <is>
           <t>2025-09-23 00:00:00</t>
         </is>
       </c>
-      <c r="L6" s="5" t="inlineStr">
+      <c r="L6" s="2" t="inlineStr">
         <is>
           <t>2025-10-07 00:00:00</t>
         </is>
       </c>
-      <c r="M6" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N6" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O6" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P6" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Q6" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R6" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S6" s="5" t="inlineStr">
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N6" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q6" s="2" t="n"/>
+      <c r="R6" s="2" t="n"/>
+      <c r="S6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
         </is>
       </c>
-      <c r="T6" s="6" t="inlineStr">
+      <c r="T6" s="3" t="inlineStr">
         <is>
           <t>21.5</t>
         </is>
       </c>
-      <c r="U6" s="7">
-        <f>V6/T6*1000</f>
-        <v/>
-      </c>
-      <c r="V6" s="8" t="inlineStr">
-        <is>
-          <t>50000.0</t>
-        </is>
-      </c>
-      <c r="W6" s="5" t="inlineStr">
+      <c r="U6" s="3" t="inlineStr">
+        <is>
+          <t>2325581.395</t>
+        </is>
+      </c>
+      <c r="V6" s="4" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="W6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Non-cancellable, but can be shifted with a 60 days notice before launch </t>
         </is>
       </c>
-      <c r="X6" s="5">
-        <f>U57/'Max Avails'!U58</f>
-        <v/>
-      </c>
-      <c r="Y6" s="5" t="inlineStr">
+      <c r="X6" s="2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Y6" s="2" t="inlineStr">
         <is>
           <t>$10K Line Item Minimum, $75K Plan Minimum</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n"/>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>7.5% ADDED VALUE + 10% Buy More Get More First Screen Rotational</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Added Value (17.5%)_Native 1st Screen Ad Rotational_Lead in/Continuity_Click to Video/App: 
 Untargeted 
@@ -1312,116 +1235,101 @@
 9/23-10/7: Click to App (2017+)</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Untargeted</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Smart TV </t>
         </is>
       </c>
-      <c r="G7" s="5" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
 Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
         </is>
       </c>
-      <c r="H7" s="5" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>Yes (but can be tracked by a DCM 1x1)</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>Added Value</t>
         </is>
       </c>
-      <c r="J7" s="5" t="inlineStr">
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>Custom Display</t>
         </is>
       </c>
-      <c r="K7" s="5" t="inlineStr">
+      <c r="K7" s="2" t="inlineStr">
         <is>
           <t>2025-09-18 00:00:00</t>
         </is>
       </c>
-      <c r="L7" s="5" t="inlineStr">
+      <c r="L7" s="2" t="inlineStr">
         <is>
           <t>2025-10-07 00:00:00</t>
         </is>
       </c>
-      <c r="M7" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="N7" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O7" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="P7" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Q7" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R7" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S7" s="5" t="inlineStr">
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N7" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O7" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P7" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q7" s="2" t="n"/>
+      <c r="R7" s="2" t="n"/>
+      <c r="S7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
         </is>
       </c>
-      <c r="T7" s="6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="U7" s="7">
-        <f>(400000*17.5%)/14.25*1000</f>
-        <v/>
-      </c>
-      <c r="V7" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="W7" s="5" t="inlineStr">
+      <c r="T7" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U7" s="3" t="inlineStr">
+        <is>
+          <t>4912280.702</t>
+        </is>
+      </c>
+      <c r="V7" s="4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W7" s="2" t="inlineStr">
         <is>
           <t>14 days</t>
         </is>
       </c>
-      <c r="X7" s="5" t="inlineStr">
+      <c r="X7" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Y7" s="5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="Y7" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>